<commit_message>
May and April Data Input
</commit_message>
<xml_diff>
--- a/RClass/InternHours.xlsx
+++ b/RClass/InternHours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophi\Documents\GitHub\TanakekeProject\RClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BD08ED-3DDB-4269-BF85-4D12A03F4200}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCA8148-7BC8-4D7E-9F10-F57C8EDCF201}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="66">
   <si>
     <t>Siapa</t>
   </si>
@@ -223,6 +223,12 @@
   </si>
   <si>
     <t>20/05/2024</t>
+  </si>
+  <si>
+    <t>APRIL</t>
+  </si>
+  <si>
+    <t>NEED TO TALK</t>
   </si>
 </sst>
 </file>
@@ -534,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -572,6 +578,7 @@
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -973,14 +980,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66BFB920-5DF5-4276-811E-D752F7CB5ECC}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="26.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -995,7 +1003,7 @@
       <c r="F1" s="29"/>
       <c r="G1" s="30"/>
       <c r="I1" s="28" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="J1" s="29"/>
       <c r="K1" s="29"/>
@@ -1257,9 +1265,15 @@
       <c r="J7" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="24"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="34"/>
+      <c r="K7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="31">
+        <v>45449</v>
+      </c>
+      <c r="M7" s="34" t="s">
+        <v>54</v>
+      </c>
       <c r="N7" s="6" t="s">
         <v>22</v>
       </c>
@@ -1329,9 +1343,15 @@
       <c r="J9" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="24"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="34"/>
+      <c r="K9" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="31">
+        <v>45443</v>
+      </c>
+      <c r="M9" s="34" t="s">
+        <v>54</v>
+      </c>
       <c r="N9" s="34" t="s">
         <v>49</v>
       </c>
@@ -1361,9 +1381,15 @@
       <c r="J10" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="K10" s="24"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="34"/>
+      <c r="K10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="31">
+        <v>45441</v>
+      </c>
+      <c r="M10" s="34" t="s">
+        <v>54</v>
+      </c>
       <c r="N10" s="34" t="s">
         <v>49</v>
       </c>
@@ -1431,13 +1457,21 @@
       <c r="J12" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="K12" s="24"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="34"/>
+      <c r="K12" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="31">
+        <v>45443</v>
+      </c>
+      <c r="M12" s="34" t="s">
+        <v>54</v>
+      </c>
       <c r="N12" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="O12" s="7"/>
+      <c r="O12" s="7" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
@@ -1465,13 +1499,21 @@
       <c r="J13" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="K13" s="24"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="6"/>
+      <c r="K13" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="35">
+        <v>45443</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="N13" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="O13" s="7"/>
+      <c r="O13" s="7" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
@@ -1497,13 +1539,21 @@
       <c r="J14" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="24"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="34"/>
+      <c r="K14" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="31">
+        <v>45443</v>
+      </c>
+      <c r="M14" s="34" t="s">
+        <v>54</v>
+      </c>
       <c r="N14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="O14" s="7"/>
+      <c r="O14" s="7" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
@@ -1534,8 +1584,8 @@
       <c r="K15" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="18" t="s">
-        <v>63</v>
+      <c r="L15" s="35">
+        <v>45432</v>
       </c>
       <c r="M15" s="6" t="s">
         <v>54</v>
@@ -1571,9 +1621,15 @@
       <c r="J16" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="K16" s="24"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="6"/>
+      <c r="K16" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="35">
+        <v>45441</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="N16" s="6" t="s">
         <v>47</v>
       </c>
@@ -1605,9 +1661,15 @@
       <c r="J17" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="K17" s="24"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="6"/>
+      <c r="K17" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="35">
+        <v>45433</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="N17" s="6" t="s">
         <v>47</v>
       </c>
@@ -1639,9 +1701,15 @@
       <c r="J18" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="K18" s="24"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="6"/>
+      <c r="K18" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="35">
+        <v>45432</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="N18" s="6" t="s">
         <v>47</v>
       </c>
@@ -1654,9 +1722,15 @@
       <c r="B19" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="6"/>
+      <c r="C19" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="35">
+        <v>45443</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="F19" s="6" t="s">
         <v>50</v>
       </c>
@@ -1667,13 +1741,21 @@
       <c r="J19" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="K19" s="24"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="6"/>
+      <c r="K19" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" s="35">
+        <v>45433</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="N19" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="O19" s="7"/>
+      <c r="O19" s="7" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="8" t="s">
@@ -1682,9 +1764,15 @@
       <c r="B20" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="9"/>
+      <c r="C20" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="37">
+        <v>45443</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="F20" s="9" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
Finish July Vids - just need to take recordings
</commit_message>
<xml_diff>
--- a/RClass/InternHours.xlsx
+++ b/RClass/InternHours.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophi\Documents\GitHub\TanakekeProject\RClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B50E3B-6F43-4324-A530-83819079AB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BBDA76-70D7-4440-8029-3CF69B1B956A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetings" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="85">
   <si>
     <t>Siapa</t>
   </si>
@@ -275,6 +275,12 @@
   </si>
   <si>
     <t>NOT SAMPLED</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>TO DO order</t>
   </si>
 </sst>
 </file>
@@ -586,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -627,6 +633,7 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1026,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66BFB920-5DF5-4276-811E-D752F7CB5ECC}">
-  <dimension ref="A1:AV20"/>
+  <dimension ref="A1:BC20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z2" workbookViewId="0">
-      <selection activeCell="AD16" sqref="AD16"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AH15" sqref="AH15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1042,9 +1049,10 @@
     <col min="27" max="27" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="28" t="s">
         <v>56</v>
       </c>
@@ -1090,26 +1098,35 @@
       <c r="AK1" s="29"/>
       <c r="AL1" s="29"/>
       <c r="AM1" s="30"/>
-      <c r="AQ1" t="s">
+      <c r="AO1" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="AP1" s="29"/>
+      <c r="AQ1" s="29"/>
+      <c r="AR1" s="29"/>
+      <c r="AS1" s="29"/>
+      <c r="AT1" s="29"/>
+      <c r="AU1" s="30"/>
+      <c r="AX1" t="s">
         <v>60</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AY1" t="s">
         <v>61</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AZ1" t="s">
         <v>70</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="BA1" t="s">
         <v>62</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="BB1" t="s">
         <v>74</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="BC1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
@@ -1201,7 +1218,7 @@
         <v>15</v>
       </c>
       <c r="AI2" s="22" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="AJ2" s="21" t="s">
         <v>17</v>
@@ -1215,26 +1232,47 @@
       <c r="AM2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="AQ2" s="27" t="s">
+      <c r="AO2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP2" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ2" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AS2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="AT2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="AU2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="AX2" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="AR2" s="27" t="s">
+      <c r="AY2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="AS2" s="27" t="s">
+      <c r="AZ2" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="AT2">
+      <c r="BA2">
         <v>10</v>
       </c>
-      <c r="AU2">
+      <c r="BB2">
         <v>300</v>
       </c>
-      <c r="AV2">
+      <c r="BC2">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -1309,31 +1347,44 @@
       <c r="AH3" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="AI3" s="23"/>
+      <c r="AI3" s="23">
+        <v>17</v>
+      </c>
       <c r="AJ3" s="32"/>
       <c r="AK3" s="33"/>
       <c r="AL3" s="3"/>
       <c r="AM3" s="4"/>
-      <c r="AQ3" s="27" t="s">
+      <c r="AO3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ3" s="23"/>
+      <c r="AR3" s="32"/>
+      <c r="AS3" s="33"/>
+      <c r="AT3" s="3"/>
+      <c r="AU3" s="4"/>
+      <c r="AX3" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="AR3" s="27" t="s">
+      <c r="AY3" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="AS3" s="27" t="s">
+      <c r="AZ3" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="AT3">
+      <c r="BA3">
         <v>9</v>
       </c>
-      <c r="AU3">
+      <c r="BB3">
         <v>300</v>
       </c>
-      <c r="AV3">
+      <c r="BC3">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>27</v>
       </c>
@@ -1408,31 +1459,44 @@
       <c r="AH4" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="AI4" s="24"/>
+      <c r="AI4" s="24">
+        <v>13</v>
+      </c>
       <c r="AJ4" s="31"/>
       <c r="AK4" s="34"/>
       <c r="AL4" s="6"/>
       <c r="AM4" s="7"/>
-      <c r="AQ4" s="27" t="s">
+      <c r="AO4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP4" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="AQ4" s="24"/>
+      <c r="AR4" s="31"/>
+      <c r="AS4" s="34"/>
+      <c r="AT4" s="6"/>
+      <c r="AU4" s="7"/>
+      <c r="AX4" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="AR4" s="27" t="s">
+      <c r="AY4" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="AS4" s="27" t="s">
+      <c r="AZ4" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="AT4">
+      <c r="BA4">
         <v>8</v>
       </c>
-      <c r="AU4">
+      <c r="BB4">
         <v>300</v>
       </c>
-      <c r="AV4">
+      <c r="BC4">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
@@ -1507,31 +1571,44 @@
       <c r="AH5" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AI5" s="24"/>
+      <c r="AI5" s="24">
+        <v>18</v>
+      </c>
       <c r="AJ5" s="31"/>
       <c r="AK5" s="34"/>
       <c r="AL5" s="6"/>
       <c r="AM5" s="7"/>
-      <c r="AQ5" s="27" t="s">
+      <c r="AO5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP5" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="AQ5" s="24"/>
+      <c r="AR5" s="31"/>
+      <c r="AS5" s="34"/>
+      <c r="AT5" s="6"/>
+      <c r="AU5" s="7"/>
+      <c r="AX5" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="AR5" s="27" t="s">
+      <c r="AY5" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="AS5" s="27" t="s">
+      <c r="AZ5" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="AT5">
+      <c r="BA5">
         <v>10</v>
       </c>
-      <c r="AU5">
+      <c r="BB5">
         <v>300</v>
       </c>
-      <c r="AV5">
+      <c r="BC5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
@@ -1612,13 +1689,26 @@
       <c r="AH6" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="AI6" s="24"/>
+      <c r="AI6" s="24">
+        <v>16</v>
+      </c>
       <c r="AJ6" s="35"/>
       <c r="AK6" s="6"/>
       <c r="AL6" s="6"/>
       <c r="AM6" s="7"/>
+      <c r="AO6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP6" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ6" s="24"/>
+      <c r="AR6" s="35"/>
+      <c r="AS6" s="6"/>
+      <c r="AT6" s="6"/>
+      <c r="AU6" s="7"/>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>27</v>
       </c>
@@ -1693,13 +1783,26 @@
       <c r="AH7" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="AI7" s="24"/>
+      <c r="AI7" s="24">
+        <v>6</v>
+      </c>
       <c r="AJ7" s="31"/>
       <c r="AK7" s="34"/>
       <c r="AL7" s="6"/>
       <c r="AM7" s="7"/>
+      <c r="AO7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP7" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ7" s="24"/>
+      <c r="AR7" s="31"/>
+      <c r="AS7" s="34"/>
+      <c r="AT7" s="6"/>
+      <c r="AU7" s="7"/>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
@@ -1776,13 +1879,26 @@
       <c r="AH8" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="AI8" s="24"/>
+      <c r="AI8" s="24">
+        <v>14</v>
+      </c>
       <c r="AJ8" s="31"/>
       <c r="AK8" s="34"/>
       <c r="AL8" s="6"/>
       <c r="AM8" s="7"/>
+      <c r="AO8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP8" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AQ8" s="24"/>
+      <c r="AR8" s="31"/>
+      <c r="AS8" s="34"/>
+      <c r="AT8" s="6"/>
+      <c r="AU8" s="7"/>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
@@ -1859,13 +1975,26 @@
       <c r="AH9" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="AI9" s="24"/>
+      <c r="AI9" s="24">
+        <v>11</v>
+      </c>
       <c r="AJ9" s="31"/>
       <c r="AK9" s="34"/>
       <c r="AL9" s="34"/>
       <c r="AM9" s="7"/>
+      <c r="AO9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP9" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ9" s="24"/>
+      <c r="AR9" s="31"/>
+      <c r="AS9" s="34"/>
+      <c r="AT9" s="34"/>
+      <c r="AU9" s="7"/>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -1940,13 +2069,26 @@
       <c r="AH10" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="AI10" s="24"/>
+      <c r="AI10" s="24">
+        <v>12</v>
+      </c>
       <c r="AJ10" s="31"/>
       <c r="AK10" s="34"/>
       <c r="AL10" s="34"/>
       <c r="AM10" s="7"/>
+      <c r="AO10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP10" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ10" s="24"/>
+      <c r="AR10" s="31"/>
+      <c r="AS10" s="34"/>
+      <c r="AT10" s="34"/>
+      <c r="AU10" s="7"/>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>27</v>
       </c>
@@ -2031,13 +2173,26 @@
       <c r="AH11" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AI11" s="25"/>
+      <c r="AI11" s="25">
+        <v>4</v>
+      </c>
       <c r="AJ11" s="38"/>
       <c r="AK11" s="15"/>
       <c r="AL11" s="15"/>
       <c r="AM11" s="16"/>
+      <c r="AO11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AQ11" s="25"/>
+      <c r="AR11" s="38"/>
+      <c r="AS11" s="15"/>
+      <c r="AT11" s="15"/>
+      <c r="AU11" s="16"/>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>37</v>
       </c>
@@ -2114,13 +2269,26 @@
       <c r="AH12" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="AI12" s="24"/>
+      <c r="AI12" s="24">
+        <v>8</v>
+      </c>
       <c r="AJ12" s="31"/>
       <c r="AK12" s="34"/>
       <c r="AL12" s="6"/>
       <c r="AM12" s="7"/>
+      <c r="AO12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP12" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ12" s="24"/>
+      <c r="AR12" s="31"/>
+      <c r="AS12" s="34"/>
+      <c r="AT12" s="6"/>
+      <c r="AU12" s="7"/>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>37</v>
       </c>
@@ -2199,13 +2367,26 @@
       <c r="AH13" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="AI13" s="24"/>
+      <c r="AI13" s="24">
+        <v>2</v>
+      </c>
       <c r="AJ13" s="35"/>
       <c r="AK13" s="6"/>
       <c r="AL13" s="6"/>
       <c r="AM13" s="7"/>
+      <c r="AO13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP13" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="AQ13" s="24"/>
+      <c r="AR13" s="35"/>
+      <c r="AS13" s="6"/>
+      <c r="AT13" s="6"/>
+      <c r="AU13" s="7"/>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -2266,9 +2447,13 @@
         <v>40</v>
       </c>
       <c r="AA14" s="24"/>
-      <c r="AB14" s="31"/>
+      <c r="AB14" s="31">
+        <v>45729</v>
+      </c>
       <c r="AC14" s="34"/>
-      <c r="AD14" s="6"/>
+      <c r="AD14" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="AE14" s="7"/>
       <c r="AG14" s="5" t="s">
         <v>37</v>
@@ -2276,13 +2461,26 @@
       <c r="AH14" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="AI14" s="24"/>
+      <c r="AI14" s="24">
+        <v>5</v>
+      </c>
       <c r="AJ14" s="31"/>
       <c r="AK14" s="34"/>
       <c r="AL14" s="6"/>
       <c r="AM14" s="7"/>
+      <c r="AO14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP14" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ14" s="24"/>
+      <c r="AR14" s="31"/>
+      <c r="AS14" s="34"/>
+      <c r="AT14" s="6"/>
+      <c r="AU14" s="7"/>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>37</v>
       </c>
@@ -2359,13 +2557,26 @@
       <c r="AH15" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="AI15" s="24"/>
+      <c r="AI15" s="24">
+        <v>1</v>
+      </c>
       <c r="AJ15" s="35"/>
       <c r="AK15" s="6"/>
       <c r="AL15" s="6"/>
       <c r="AM15" s="7"/>
+      <c r="AO15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP15" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ15" s="24"/>
+      <c r="AR15" s="35"/>
+      <c r="AS15" s="6"/>
+      <c r="AT15" s="6"/>
+      <c r="AU15" s="7"/>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>37</v>
       </c>
@@ -2442,13 +2653,26 @@
       <c r="AH16" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="AI16" s="24"/>
+      <c r="AI16" s="24">
+        <v>15</v>
+      </c>
       <c r="AJ16" s="35"/>
       <c r="AK16" s="6"/>
       <c r="AL16" s="6"/>
       <c r="AM16" s="7"/>
+      <c r="AO16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP16" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="AQ16" s="24"/>
+      <c r="AR16" s="35"/>
+      <c r="AS16" s="6"/>
+      <c r="AT16" s="6"/>
+      <c r="AU16" s="7"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>37</v>
       </c>
@@ -2523,13 +2747,26 @@
       <c r="AH17" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="AI17" s="24"/>
+      <c r="AI17" s="24">
+        <v>7</v>
+      </c>
       <c r="AJ17" s="35"/>
       <c r="AK17" s="6"/>
       <c r="AL17" s="6"/>
       <c r="AM17" s="7"/>
+      <c r="AO17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP17" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ17" s="24"/>
+      <c r="AR17" s="35"/>
+      <c r="AS17" s="6"/>
+      <c r="AT17" s="6"/>
+      <c r="AU17" s="7"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
@@ -2608,13 +2845,26 @@
       <c r="AH18" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="AI18" s="24"/>
+      <c r="AI18" s="24">
+        <v>10</v>
+      </c>
       <c r="AJ18" s="35"/>
       <c r="AK18" s="6"/>
       <c r="AL18" s="6"/>
       <c r="AM18" s="7"/>
+      <c r="AO18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP18" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ18" s="24"/>
+      <c r="AR18" s="35"/>
+      <c r="AS18" s="6"/>
+      <c r="AT18" s="6"/>
+      <c r="AU18" s="7"/>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>37</v>
       </c>
@@ -2693,13 +2943,26 @@
       <c r="AH19" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="AI19" s="24"/>
+      <c r="AI19" s="24">
+        <v>9</v>
+      </c>
       <c r="AJ19" s="35"/>
       <c r="AK19" s="6"/>
       <c r="AL19" s="6"/>
       <c r="AM19" s="7"/>
+      <c r="AO19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP19" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ19" s="24"/>
+      <c r="AR19" s="35"/>
+      <c r="AS19" s="6"/>
+      <c r="AT19" s="6"/>
+      <c r="AU19" s="7"/>
     </row>
-    <row r="20" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:47" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="8" t="s">
         <v>37</v>
       </c>
@@ -2764,9 +3027,13 @@
         <v>46</v>
       </c>
       <c r="AA20" s="26"/>
-      <c r="AB20" s="20"/>
+      <c r="AB20" s="40">
+        <v>45729</v>
+      </c>
       <c r="AC20" s="9"/>
-      <c r="AD20" s="9"/>
+      <c r="AD20" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="AE20" s="10"/>
       <c r="AG20" s="8" t="s">
         <v>37</v>
@@ -2774,11 +3041,24 @@
       <c r="AH20" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="AI20" s="26"/>
+      <c r="AI20" s="26">
+        <v>3</v>
+      </c>
       <c r="AJ20" s="20"/>
       <c r="AK20" s="9"/>
       <c r="AL20" s="9"/>
       <c r="AM20" s="10"/>
+      <c r="AO20" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP20" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ20" s="26"/>
+      <c r="AR20" s="20"/>
+      <c r="AS20" s="9"/>
+      <c r="AT20" s="9"/>
+      <c r="AU20" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>